<commit_message>
finishe the single variable regression
</commit_message>
<xml_diff>
--- a/data/areas.xlsx
+++ b/data/areas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\programming folder\computer science and stocks\machine learning\thoery_of_ml\project_one\linearRegression\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C820881A-05A5-4250-B89B-39731AE65F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3173935B-0F3F-49A7-8EF7-254870D33E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="2180" windowWidth="14400" windowHeight="7270" xr2:uid="{0F003BBC-7A4D-498B-B408-0C1F1BAD007D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{0F003BBC-7A4D-498B-B408-0C1F1BAD007D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,40 +379,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A845D30-C299-44F5-B765-2BFBB6E8046C}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="B1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>20003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>30885</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>39954</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>345245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>244444</v>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>3203</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>4003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>